<commit_message>
fix transmission and sets files
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/Data_EMPIRE-Public/Transmission.xlsx
+++ b/EMPIRE_extension/Data_EMPIRE-Public/Transmission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gorandurakovic/EMPIRE-Wind_North_Sea/Data handler/hydrogenAllCountries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivergjorvad/Desktop/prosjektoppgave/EMPIRE_extension/Data_EMPIRE-Public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D41A3EE2-8C1D-5344-A9A6-7516B4A430F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5318FC-86C7-4D49-9444-3431E6F2513D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="680" windowWidth="28800" windowHeight="16340" tabRatio="804" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="804" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lineEfficiency" sheetId="9" r:id="rId1"/>
@@ -443,10 +443,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -19248,7 +19247,7 @@
       <c r="C1094">
         <v>4</v>
       </c>
-      <c r="D1094" s="5">
+      <c r="D1094" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -20746,7 +20745,7 @@
       <c r="C1201">
         <v>5</v>
       </c>
-      <c r="D1201" s="5">
+      <c r="D1201" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -22244,7 +22243,7 @@
       <c r="C1308">
         <v>6</v>
       </c>
-      <c r="D1308" s="5">
+      <c r="D1308" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -23742,7 +23741,7 @@
       <c r="C1415">
         <v>7</v>
       </c>
-      <c r="D1415" s="5">
+      <c r="D1415" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -25240,7 +25239,7 @@
       <c r="C1522">
         <v>8</v>
       </c>
-      <c r="D1522" s="5">
+      <c r="D1522" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -32596,11 +32595,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAE27BA-DAF9-49AB-B8A1-9EA6D16D2140}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G227" sqref="G227"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32615,12 +32613,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -32631,7 +32629,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -32642,7 +32640,7 @@
         <v>355.58387909599998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -32653,7 +32651,7 @@
         <v>253.34554350939999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -32664,7 +32662,7 @@
         <v>490.12429992760002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -32675,7 +32673,7 @@
         <v>338.3496671533</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -32686,7 +32684,7 @@
         <v>485.9159178264</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -32697,7 +32695,7 @@
         <v>151.36996057179999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -32708,7 +32706,7 @@
         <v>190.5919036125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -32719,7 +32717,7 @@
         <v>190.298459399</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -32730,7 +32728,7 @@
         <v>444.65858714759997</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -32741,7 +32739,7 @@
         <v>129.0493737912</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -32752,7 +32750,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -32763,7 +32761,7 @@
         <v>427.94306233250001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -32774,7 +32772,7 @@
         <v>269.5376549673</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -32785,7 +32783,7 @@
         <v>395.00762258190002</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -32796,7 +32794,7 @@
         <v>311.5642925532</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -32807,7 +32805,7 @@
         <v>579.15627342810001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -32818,7 +32816,7 @@
         <v>317.56030664690002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -32829,7 +32827,7 @@
         <v>498.49053630039998</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -32840,7 +32838,7 @@
         <v>336.40332772599999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -32851,7 +32849,7 @@
         <v>338.47352159000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -32862,7 +32860,7 @@
         <v>208.04557377270001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -32873,7 +32871,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -32884,7 +32882,7 @@
         <v>766.47990591270002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -32895,7 +32893,7 @@
         <v>396.45512374790002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -32906,7 +32904,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -32917,7 +32915,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -32928,7 +32926,7 @@
         <v>450.09249860360001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -32939,7 +32937,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -32950,7 +32948,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -32961,7 +32959,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -32972,7 +32970,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -32983,7 +32981,7 @@
         <v>196.72414130889999</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -32994,7 +32992,7 @@
         <v>792.91024749589997</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -33005,7 +33003,7 @@
         <v>339.00970126940001</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -33016,7 +33014,7 @@
         <v>757.97501126400005</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -33027,7 +33025,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -33038,7 +33036,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -33060,7 +33058,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -33071,7 +33069,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -33082,7 +33080,7 @@
         <v>275.78893137969999</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -33093,7 +33091,7 @@
         <v>243.67570924770001</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -33104,7 +33102,7 @@
         <v>335.82138652809999</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -33115,7 +33113,7 @@
         <v>127.74361297900001</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -33126,7 +33124,7 @@
         <v>335.69655359400002</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -33137,7 +33135,7 @@
         <v>370.06253786939999</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -33148,7 +33146,7 @@
         <v>152.19838247409999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -33159,7 +33157,7 @@
         <v>368.13205986930001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -33170,7 +33168,7 @@
         <v>204.18187291300001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -33181,7 +33179,7 @@
         <v>204.04497589939999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -33192,7 +33190,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -33203,7 +33201,7 @@
         <v>325.68358765839997</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -33214,7 +33212,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -33225,7 +33223,7 @@
         <v>360.42303940750003</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -33236,7 +33234,7 @@
         <v>359.21936093430003</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -33247,7 +33245,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -33258,7 +33256,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -33269,7 +33267,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -33280,7 +33278,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -33291,7 +33289,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -33302,7 +33300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -33313,7 +33311,7 @@
         <v>402.88719079123115</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -33324,7 +33322,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -33335,7 +33333,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -33346,7 +33344,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>21</v>
       </c>
@@ -33357,7 +33355,7 @@
         <v>357.66743167118716</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -33368,7 +33366,7 @@
         <v>467.34821614854997</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -33379,7 +33377,7 @@
         <v>847.5603817319942</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -33390,7 +33388,7 @@
         <v>918.59482578760696</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -33401,7 +33399,7 @@
         <v>236.85249023743398</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>22</v>
       </c>
@@ -33434,7 +33432,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -33445,7 +33443,7 @@
         <v>394.32505737533904</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -33456,7 +33454,7 @@
         <v>481.95284790319215</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -33467,7 +33465,7 @@
         <v>350.51116211141249</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -33478,7 +33476,7 @@
         <v>406.79208404593203</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -33489,7 +33487,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -33500,7 +33498,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -33511,7 +33509,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -33522,7 +33520,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>34</v>
       </c>
@@ -33533,7 +33531,7 @@
         <v>325.68358765839997</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -33544,7 +33542,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -33555,7 +33553,7 @@
         <v>325.68358765839997</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -33566,7 +33564,7 @@
         <v>325.68358765839997</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>75</v>
       </c>
@@ -33577,7 +33575,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -33588,7 +33586,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -33599,7 +33597,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -33610,7 +33608,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -33621,7 +33619,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -33632,7 +33630,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>82</v>
       </c>
@@ -33643,7 +33641,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>83</v>
       </c>
@@ -33654,7 +33652,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>84</v>
       </c>
@@ -33665,7 +33663,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -33676,7 +33674,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>86</v>
       </c>
@@ -33687,7 +33685,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -33698,7 +33696,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>88</v>
       </c>
@@ -33709,7 +33707,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>77</v>
       </c>
@@ -33720,7 +33718,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>78</v>
       </c>
@@ -33731,7 +33729,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>79</v>
       </c>
@@ -33742,7 +33740,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>80</v>
       </c>
@@ -33753,7 +33751,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>81</v>
       </c>
@@ -33764,7 +33762,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>82</v>
       </c>
@@ -33775,7 +33773,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>83</v>
       </c>
@@ -33786,7 +33784,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>84</v>
       </c>
@@ -33797,7 +33795,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>85</v>
       </c>
@@ -33808,7 +33806,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>86</v>
       </c>
@@ -33819,7 +33817,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -33830,7 +33828,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>88</v>
       </c>
@@ -33841,7 +33839,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>78</v>
       </c>
@@ -33852,7 +33850,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>79</v>
       </c>
@@ -33863,7 +33861,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>80</v>
       </c>
@@ -33874,7 +33872,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>81</v>
       </c>
@@ -33885,7 +33883,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>82</v>
       </c>
@@ -33896,7 +33894,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>83</v>
       </c>
@@ -33907,7 +33905,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>84</v>
       </c>
@@ -33918,7 +33916,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>85</v>
       </c>
@@ -33929,7 +33927,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>86</v>
       </c>
@@ -33940,7 +33938,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>87</v>
       </c>
@@ -33951,7 +33949,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>88</v>
       </c>
@@ -33962,7 +33960,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>79</v>
       </c>
@@ -33973,7 +33971,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>80</v>
       </c>
@@ -33984,7 +33982,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>81</v>
       </c>
@@ -33995,7 +33993,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>82</v>
       </c>
@@ -34006,7 +34004,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>83</v>
       </c>
@@ -34017,7 +34015,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>84</v>
       </c>
@@ -34028,7 +34026,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>85</v>
       </c>
@@ -34039,7 +34037,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>86</v>
       </c>
@@ -34050,7 +34048,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>87</v>
       </c>
@@ -34061,7 +34059,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>88</v>
       </c>
@@ -34072,7 +34070,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>80</v>
       </c>
@@ -34083,7 +34081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>81</v>
       </c>
@@ -34094,7 +34092,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>82</v>
       </c>
@@ -34105,7 +34103,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>83</v>
       </c>
@@ -34116,7 +34114,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>84</v>
       </c>
@@ -34127,7 +34125,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>85</v>
       </c>
@@ -34138,7 +34136,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>86</v>
       </c>
@@ -34149,7 +34147,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>87</v>
       </c>
@@ -34160,7 +34158,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -34171,7 +34169,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>81</v>
       </c>
@@ -34182,7 +34180,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>82</v>
       </c>
@@ -34193,7 +34191,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>83</v>
       </c>
@@ -34204,7 +34202,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>84</v>
       </c>
@@ -34215,7 +34213,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>85</v>
       </c>
@@ -34226,7 +34224,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>86</v>
       </c>
@@ -34237,7 +34235,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>87</v>
       </c>
@@ -34248,7 +34246,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -34259,7 +34257,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>82</v>
       </c>
@@ -34270,7 +34268,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>83</v>
       </c>
@@ -34281,7 +34279,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>84</v>
       </c>
@@ -34292,7 +34290,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>85</v>
       </c>
@@ -34303,7 +34301,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>86</v>
       </c>
@@ -34314,7 +34312,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>87</v>
       </c>
@@ -34325,7 +34323,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>88</v>
       </c>
@@ -34336,7 +34334,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>83</v>
       </c>
@@ -34347,7 +34345,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>84</v>
       </c>
@@ -34358,7 +34356,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>85</v>
       </c>
@@ -34369,7 +34367,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>86</v>
       </c>
@@ -34380,7 +34378,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>87</v>
       </c>
@@ -34391,7 +34389,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>88</v>
       </c>
@@ -34402,7 +34400,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>84</v>
       </c>
@@ -34413,7 +34411,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>85</v>
       </c>
@@ -34424,7 +34422,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>86</v>
       </c>
@@ -34435,7 +34433,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>87</v>
       </c>
@@ -34446,7 +34444,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>88</v>
       </c>
@@ -34457,7 +34455,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>85</v>
       </c>
@@ -34468,7 +34466,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>86</v>
       </c>
@@ -34479,7 +34477,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>87</v>
       </c>
@@ -34490,7 +34488,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>88</v>
       </c>
@@ -34501,7 +34499,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>86</v>
       </c>
@@ -34512,7 +34510,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>87</v>
       </c>
@@ -34523,7 +34521,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>88</v>
       </c>
@@ -34534,7 +34532,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>87</v>
       </c>
@@ -34545,7 +34543,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>88</v>
       </c>
@@ -34556,7 +34554,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>88</v>
       </c>
@@ -34567,7 +34565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>76</v>
       </c>
@@ -34578,7 +34576,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>75</v>
       </c>
@@ -34589,7 +34587,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>77</v>
       </c>
@@ -34600,7 +34598,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>78</v>
       </c>
@@ -34611,7 +34609,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>79</v>
       </c>
@@ -34622,7 +34620,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>80</v>
       </c>
@@ -34633,7 +34631,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>81</v>
       </c>
@@ -34644,7 +34642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>82</v>
       </c>
@@ -34655,7 +34653,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>82</v>
       </c>
@@ -34666,7 +34664,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>83</v>
       </c>
@@ -34677,7 +34675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>84</v>
       </c>
@@ -34688,7 +34686,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>84</v>
       </c>
@@ -34699,7 +34697,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>85</v>
       </c>
@@ -34710,7 +34708,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>86</v>
       </c>
@@ -34721,7 +34719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>87</v>
       </c>
@@ -34732,7 +34730,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>88</v>
       </c>
@@ -34743,7 +34741,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -34754,7 +34752,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>89</v>
       </c>
@@ -34765,7 +34763,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>89</v>
       </c>
@@ -34776,7 +34774,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>89</v>
       </c>
@@ -34787,7 +34785,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>89</v>
       </c>
@@ -34798,7 +34796,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>89</v>
       </c>
@@ -34809,7 +34807,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -34820,7 +34818,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>89</v>
       </c>
@@ -34831,7 +34829,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>89</v>
       </c>
@@ -34842,7 +34840,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>89</v>
       </c>
@@ -34853,7 +34851,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>89</v>
       </c>
@@ -34864,7 +34862,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>89</v>
       </c>
@@ -34875,7 +34873,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>89</v>
       </c>
@@ -34886,7 +34884,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>89</v>
       </c>
@@ -34897,7 +34895,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>89</v>
       </c>
@@ -34908,7 +34906,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>89</v>
       </c>
@@ -34919,7 +34917,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>89</v>
       </c>
@@ -34930,7 +34928,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>89</v>
       </c>
@@ -34941,7 +34939,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>89</v>
       </c>
@@ -34952,7 +34950,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>89</v>
       </c>
@@ -34963,7 +34961,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>89</v>
       </c>
@@ -34975,13 +34973,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C216" xr:uid="{70B7885A-5FE4-4619-A9B2-A463CA2536DA}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Ireland"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C216" xr:uid="{70B7885A-5FE4-4619-A9B2-A463CA2536DA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -35009,10 +35001,10 @@
       <c r="A1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -35020,10 +35012,10 @@
       <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -35037,10 +35029,10 @@
       <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -35054,10 +35046,10 @@
       <c r="C4">
         <v>661.609375</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -35071,10 +35063,10 @@
       <c r="C5">
         <v>661.609375</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -35092,10 +35084,10 @@
         <f>C6/C5</f>
         <v>0.91363389462248779</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -35706,7 +35698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D811"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -47945,10 +47937,10 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
+      <c r="A81" t="s">
         <v>33</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" t="s">
         <v>35</v>
       </c>
       <c r="C81">
@@ -47956,10 +47948,10 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="A82" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" t="s">
         <v>35</v>
       </c>
       <c r="C82">
@@ -47967,10 +47959,10 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="A83" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" t="s">
         <v>35</v>
       </c>
       <c r="C83">
@@ -47978,10 +47970,10 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
         <v>37</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" t="s">
         <v>33</v>
       </c>
       <c r="C84">
@@ -47989,10 +47981,10 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+      <c r="A85" t="s">
         <v>34</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" t="s">
         <v>36</v>
       </c>
       <c r="C85">
@@ -48000,10 +47992,10 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
+      <c r="A86" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" t="s">
         <v>36</v>
       </c>
       <c r="C86">
@@ -48011,10 +48003,10 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+      <c r="A87" t="s">
         <v>22</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" t="s">
         <v>36</v>
       </c>
       <c r="C87">
@@ -48022,10 +48014,10 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>22</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" t="s">
         <v>34</v>
       </c>
       <c r="C88">

</xml_diff>